<commit_message>
Updated for DA 6833 Assignment #2 Part 2
</commit_message>
<xml_diff>
--- a/starter-analysis-exercise/data/raw-data/exampledata2.xlsx
+++ b/starter-analysis-exercise/data/raw-data/exampledata2.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27628"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27726"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{4833F394-1ECC-4F1C-86E0-04E0694934E1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CFE49E44-793D-4034-9C78-85CB830125ED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="24240" windowHeight="13740" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1536" yWindow="1536" windowWidth="17280" windowHeight="10656" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Data" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="28">
   <si>
     <t>Height</t>
   </si>
@@ -71,15 +71,9 @@
     <t>identified gender (male/female/other)</t>
   </si>
   <si>
-    <t>Shoe size</t>
-  </si>
-  <si>
     <t>Measured in ft</t>
   </si>
   <si>
-    <t>Eye Ccolor</t>
-  </si>
-  <si>
     <t>R</t>
   </si>
   <si>
@@ -101,13 +95,16 @@
     <t>Y</t>
   </si>
   <si>
-    <t>Eye Color</t>
-  </si>
-  <si>
     <t>G/R/BR/ B/Y/H/BL/O</t>
   </si>
   <si>
     <t xml:space="preserve">Eye colors( Green/ Red/ Brown/ Black/ Yellow/ Hazel/ Blue/ Orange </t>
+  </si>
+  <si>
+    <t>ShoeSize</t>
+  </si>
+  <si>
+    <t>EyeColor</t>
   </si>
 </sst>
 </file>
@@ -437,12 +434,12 @@
   <dimension ref="A1:E15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E15" sqref="E15"/>
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -453,13 +450,13 @@
         <v>14</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>16</v>
+        <v>26</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>180</v>
       </c>
@@ -473,10 +470,10 @@
         <v>12</v>
       </c>
       <c r="E2" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>175</v>
       </c>
@@ -490,10 +487,10 @@
         <v>10</v>
       </c>
       <c r="E3" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>60</v>
       </c>
@@ -507,10 +504,10 @@
         <v>8</v>
       </c>
       <c r="E4" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>178</v>
       </c>
@@ -524,10 +521,10 @@
         <v>15</v>
       </c>
       <c r="E5" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>192</v>
       </c>
@@ -544,7 +541,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>6</v>
       </c>
@@ -558,10 +555,10 @@
         <v>13</v>
       </c>
       <c r="E7" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>156</v>
       </c>
@@ -575,10 +572,10 @@
         <v>5</v>
       </c>
       <c r="E8" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>166</v>
       </c>
@@ -592,10 +589,10 @@
         <v>7</v>
       </c>
       <c r="E9" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>155</v>
       </c>
@@ -609,10 +606,10 @@
         <v>9</v>
       </c>
       <c r="E10" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>145</v>
       </c>
@@ -626,10 +623,10 @@
         <v>11</v>
       </c>
       <c r="E11" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>165</v>
       </c>
@@ -643,10 +640,10 @@
         <v>13</v>
       </c>
       <c r="E12" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>133</v>
       </c>
@@ -660,10 +657,10 @@
         <v>10</v>
       </c>
       <c r="E13" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>166</v>
       </c>
@@ -677,10 +674,10 @@
         <v>11</v>
       </c>
       <c r="E14" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>154</v>
       </c>
@@ -694,7 +691,7 @@
         <v>8</v>
       </c>
       <c r="E15" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
     </row>
   </sheetData>
@@ -707,17 +704,17 @@
   <dimension ref="A1:C6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="14.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="63.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="21.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="63.5546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="21.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>5</v>
       </c>
@@ -728,7 +725,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -739,7 +736,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -750,7 +747,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>14</v>
       </c>
@@ -761,26 +758,26 @@
         <v>13</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
+        <v>26</v>
+      </c>
+      <c r="B5" t="s">
         <v>16</v>
-      </c>
-      <c r="B5" t="s">
-        <v>17</v>
       </c>
       <c r="C5" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B6" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="C6" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
     </row>
   </sheetData>

</xml_diff>